<commit_message>
weitere änderungen bei approx
</commit_message>
<xml_diff>
--- a/INPUT_LKW.xlsx
+++ b/INPUT_LKW.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JonasSchneider/Documents/Sonstiges/Git/Projektmodul_Energiesystemische_Forschung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E17CDB-D67E-8D4D-8A5E-EE3267A087F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13519837-22A8-1A40-ADA2-0AC5D9BAA3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="4080" windowWidth="28800" windowHeight="17520" xr2:uid="{FC67FF9C-3AC7-7845-BEED-22DCFC5538A9}"/>
+    <workbookView xWindow="-400" yWindow="2760" windowWidth="38400" windowHeight="21100" xr2:uid="{FC67FF9C-3AC7-7845-BEED-22DCFC5538A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
   <si>
     <t>Ankunftszeit</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>HPC</t>
+  </si>
+  <si>
+    <t>Ladezeit</t>
   </si>
 </sst>
 </file>
@@ -405,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB74BDBC-C0B4-D94F-BDB9-A9C062B1C087}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -426,11 +429,14 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <f ca="1">ROUNDUP(RAND() * 40 / 5, 0) * 5</f>
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2">
         <f ca="1">ROUNDUP((RAND() * (800-400) + 400) / 100, 0) * 100</f>
@@ -438,13 +444,16 @@
       </c>
       <c r="C2">
         <f ca="1">ROUNDUP(RAND() * (25-10) + 10, 0)</f>
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <f t="shared" ref="A3:A11" ca="1" si="0">ROUNDUP(RAND() * 40 / 5, 0) * 5</f>
         <v>5</v>
@@ -455,135 +464,159 @@
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C11" ca="1" si="2">ROUNDUP(RAND() * (25-10) + 10, 0)</f>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ca="1" si="0"/>
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="1"/>
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="2"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="1"/>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="2"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" ca="1" si="0"/>
         <v>10</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="1"/>
-        <v>700</v>
+        <v>600</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="2"/>
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="1"/>
-        <v>500</v>
+        <v>600</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="2"/>
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="1"/>
-        <v>600</v>
+        <v>700</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="2"/>
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="1"/>
-        <v>700</v>
+        <v>800</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="2"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="1"/>
-        <v>500</v>
+        <v>800</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="2"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="1"/>
@@ -591,10 +624,13 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="2"/>
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>